<commit_message>
Add reporte 1M MP1
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56ACAF2E-32F1-4B33-9190-4C3FABEE7E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461D13D0-FC37-47D5-BAF3-31A5B892A692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>Goal</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Entrega informe final</t>
+  </si>
+  <si>
+    <t>javier.molina.ferreiro@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -750,9 +753,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -854,12 +854,58 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="7" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="2" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -875,51 +921,8 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="7" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="2" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -938,6 +941,121 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="35">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1188,121 +1306,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.249977111117893"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1583,7 +1586,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2" val="14"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1700,7 +1703,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G30" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B9:G30" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1710,12 +1713,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Descripción de la tarea" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Categoría" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Asignada a" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progreso" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Inicio" dataDxfId="15" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Días" dataDxfId="14" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Descripción de la tarea" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Categoría" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Asignada a" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progreso" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Inicio" dataDxfId="1" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Días" dataDxfId="0" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2004,17 +2007,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.4">
-      <c r="D1" s="70"/>
+      <c r="D1" s="69"/>
     </row>
     <row r="2" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="81" t="s">
+      <c r="B2" s="75"/>
+      <c r="C2" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="76"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2025,11 +2028,11 @@
     </row>
     <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -2040,13 +2043,13 @@
     </row>
     <row r="4" spans="1:13" s="8" customFormat="1" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="82" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="71"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -2057,13 +2060,13 @@
     </row>
     <row r="5" spans="1:13" s="8" customFormat="1" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="82" t="s">
+      <c r="B5" s="70"/>
+      <c r="C5" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="71"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -2074,11 +2077,11 @@
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
     </row>
     <row r="7" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -2164,8 +2167,8 @@
   </sheetPr>
   <dimension ref="A1:BP41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2186,71 +2189,71 @@
     <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="103"/>
-      <c r="AA2" s="103"/>
-      <c r="AB2" s="103"/>
-      <c r="AC2" s="103"/>
-      <c r="AD2" s="103"/>
-      <c r="AE2" s="103"/>
-      <c r="AF2" s="103"/>
-      <c r="AG2" s="103"/>
-      <c r="AH2" s="103"/>
-      <c r="AI2" s="102"/>
-      <c r="AJ2" s="102"/>
-      <c r="AK2" s="102"/>
-      <c r="AL2" s="102"/>
-      <c r="AM2" s="102"/>
-      <c r="AN2" s="102"/>
-      <c r="AO2" s="102"/>
-      <c r="AP2" s="102"/>
-      <c r="AQ2" s="102"/>
-      <c r="AR2" s="102"/>
-      <c r="AS2" s="102"/>
-      <c r="AT2" s="102"/>
-      <c r="AU2" s="102"/>
-      <c r="AV2" s="102"/>
-      <c r="AW2" s="102"/>
-      <c r="AX2" s="102"/>
-      <c r="AY2" s="102"/>
-      <c r="AZ2" s="102"/>
-      <c r="BA2" s="102"/>
-      <c r="BB2" s="102"/>
-      <c r="BC2" s="102"/>
-      <c r="BD2" s="102"/>
-      <c r="BE2" s="102"/>
-      <c r="BF2" s="102"/>
-      <c r="BG2" s="102"/>
-      <c r="BH2" s="102"/>
-      <c r="BI2" s="102"/>
-      <c r="BJ2" s="102"/>
-      <c r="BK2" s="102"/>
-      <c r="BL2" s="102"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="95"/>
+      <c r="AA2" s="95"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="95"/>
+      <c r="AD2" s="95"/>
+      <c r="AE2" s="95"/>
+      <c r="AF2" s="95"/>
+      <c r="AG2" s="95"/>
+      <c r="AH2" s="95"/>
+      <c r="AI2" s="92"/>
+      <c r="AJ2" s="92"/>
+      <c r="AK2" s="92"/>
+      <c r="AL2" s="92"/>
+      <c r="AM2" s="92"/>
+      <c r="AN2" s="92"/>
+      <c r="AO2" s="92"/>
+      <c r="AP2" s="92"/>
+      <c r="AQ2" s="92"/>
+      <c r="AR2" s="92"/>
+      <c r="AS2" s="92"/>
+      <c r="AT2" s="92"/>
+      <c r="AU2" s="92"/>
+      <c r="AV2" s="92"/>
+      <c r="AW2" s="92"/>
+      <c r="AX2" s="92"/>
+      <c r="AY2" s="92"/>
+      <c r="AZ2" s="92"/>
+      <c r="BA2" s="92"/>
+      <c r="BB2" s="92"/>
+      <c r="BC2" s="92"/>
+      <c r="BD2" s="92"/>
+      <c r="BE2" s="92"/>
+      <c r="BF2" s="92"/>
+      <c r="BG2" s="92"/>
+      <c r="BH2" s="92"/>
+      <c r="BI2" s="92"/>
+      <c r="BJ2" s="92"/>
+      <c r="BK2" s="92"/>
+      <c r="BL2" s="92"/>
       <c r="BM2" s="28"/>
     </row>
     <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2262,63 +2265,63 @@
       <c r="F3" s="32"/>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="48"/>
-      <c r="AC3" s="48"/>
-      <c r="AD3" s="48"/>
-      <c r="AE3" s="48"/>
-      <c r="AF3" s="48"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AM3" s="48"/>
-      <c r="AN3" s="48"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="48"/>
-      <c r="AR3" s="48"/>
-      <c r="AS3" s="48"/>
-      <c r="AT3" s="48"/>
-      <c r="AU3" s="48"/>
-      <c r="AV3" s="48"/>
-      <c r="AW3" s="48"/>
-      <c r="AX3" s="48"/>
-      <c r="AY3" s="48"/>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="48"/>
-      <c r="BL3" s="48"/>
-      <c r="BM3" s="49"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
+      <c r="AG3" s="47"/>
+      <c r="AH3" s="47"/>
+      <c r="AI3" s="47"/>
+      <c r="AJ3" s="47"/>
+      <c r="AK3" s="47"/>
+      <c r="AL3" s="47"/>
+      <c r="AM3" s="47"/>
+      <c r="AN3" s="47"/>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="47"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="47"/>
+      <c r="AT3" s="47"/>
+      <c r="AU3" s="47"/>
+      <c r="AV3" s="47"/>
+      <c r="AW3" s="47"/>
+      <c r="AX3" s="47"/>
+      <c r="AY3" s="47"/>
+      <c r="AZ3" s="47"/>
+      <c r="BA3" s="47"/>
+      <c r="BB3" s="47"/>
+      <c r="BC3" s="47"/>
+      <c r="BD3" s="47"/>
+      <c r="BE3" s="47"/>
+      <c r="BF3" s="47"/>
+      <c r="BG3" s="47"/>
+      <c r="BH3" s="47"/>
+      <c r="BI3" s="47"/>
+      <c r="BJ3" s="47"/>
+      <c r="BK3" s="47"/>
+      <c r="BL3" s="47"/>
+      <c r="BM3" s="48"/>
     </row>
     <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
@@ -2327,150 +2330,150 @@
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="35"/>
-      <c r="E4" s="88" t="s">
+      <c r="E4" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="85" t="s">
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="86" t="s">
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="87" t="s">
+      <c r="O4" s="101"/>
+      <c r="P4" s="101"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="83" t="s">
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="83"/>
-      <c r="AB4" s="49"/>
-      <c r="AC4" s="84" t="s">
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="AD4" s="84"/>
-      <c r="AE4" s="84"/>
-      <c r="AF4" s="84"/>
-      <c r="AG4" s="49"/>
-      <c r="AH4" s="49"/>
-      <c r="AI4" s="49"/>
-      <c r="AJ4" s="49"/>
-      <c r="AK4" s="49"/>
-      <c r="AL4" s="49"/>
-      <c r="AM4" s="49"/>
-      <c r="AN4" s="49"/>
-      <c r="AO4" s="49"/>
-      <c r="AP4" s="49"/>
-      <c r="AQ4" s="49"/>
-      <c r="AR4" s="49"/>
-      <c r="AS4" s="49"/>
-      <c r="AT4" s="49"/>
-      <c r="AU4" s="49"/>
-      <c r="AV4" s="49"/>
-      <c r="AW4" s="49"/>
-      <c r="AX4" s="49"/>
-      <c r="AY4" s="49"/>
-      <c r="AZ4" s="49"/>
-      <c r="BA4" s="49"/>
-      <c r="BB4" s="49"/>
-      <c r="BC4" s="49"/>
-      <c r="BD4" s="49"/>
-      <c r="BE4" s="49"/>
-      <c r="BF4" s="49"/>
-      <c r="BG4" s="49"/>
-      <c r="BH4" s="49"/>
-      <c r="BI4" s="49"/>
-      <c r="BJ4" s="49"/>
-      <c r="BK4" s="49"/>
-      <c r="BL4" s="49"/>
-      <c r="BM4" s="49"/>
+      <c r="AD4" s="99"/>
+      <c r="AE4" s="99"/>
+      <c r="AF4" s="99"/>
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="48"/>
+      <c r="AK4" s="48"/>
+      <c r="AL4" s="48"/>
+      <c r="AM4" s="48"/>
+      <c r="AN4" s="48"/>
+      <c r="AO4" s="48"/>
+      <c r="AP4" s="48"/>
+      <c r="AQ4" s="48"/>
+      <c r="AR4" s="48"/>
+      <c r="AS4" s="48"/>
+      <c r="AT4" s="48"/>
+      <c r="AU4" s="48"/>
+      <c r="AV4" s="48"/>
+      <c r="AW4" s="48"/>
+      <c r="AX4" s="48"/>
+      <c r="AY4" s="48"/>
+      <c r="AZ4" s="48"/>
+      <c r="BA4" s="48"/>
+      <c r="BB4" s="48"/>
+      <c r="BC4" s="48"/>
+      <c r="BD4" s="48"/>
+      <c r="BE4" s="48"/>
+      <c r="BF4" s="48"/>
+      <c r="BG4" s="48"/>
+      <c r="BH4" s="48"/>
+      <c r="BI4" s="48"/>
+      <c r="BJ4" s="48"/>
+      <c r="BK4" s="48"/>
+      <c r="BL4" s="48"/>
+      <c r="BM4" s="48"/>
     </row>
     <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
       <c r="H5" s="38"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="48"/>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="48"/>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="48"/>
-      <c r="AD5" s="48"/>
-      <c r="AE5" s="48"/>
-      <c r="AF5" s="48"/>
-      <c r="AG5" s="48"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="48"/>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="48"/>
-      <c r="AN5" s="48"/>
-      <c r="AO5" s="48"/>
-      <c r="AP5" s="48"/>
-      <c r="AQ5" s="48"/>
-      <c r="AR5" s="48"/>
-      <c r="AS5" s="48"/>
-      <c r="AT5" s="48"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="48"/>
-      <c r="AW5" s="48"/>
-      <c r="AX5" s="48"/>
-      <c r="AY5" s="48"/>
-      <c r="AZ5" s="48"/>
-      <c r="BA5" s="48"/>
-      <c r="BB5" s="48"/>
-      <c r="BC5" s="48"/>
-      <c r="BD5" s="48"/>
-      <c r="BE5" s="48"/>
-      <c r="BF5" s="48"/>
-      <c r="BG5" s="48"/>
-      <c r="BH5" s="48"/>
-      <c r="BI5" s="48"/>
-      <c r="BJ5" s="48"/>
-      <c r="BK5" s="48"/>
-      <c r="BL5" s="48"/>
-      <c r="BM5" s="49"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="47"/>
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="47"/>
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="47"/>
+      <c r="AZ5" s="47"/>
+      <c r="BA5" s="47"/>
+      <c r="BB5" s="47"/>
+      <c r="BC5" s="47"/>
+      <c r="BD5" s="47"/>
+      <c r="BE5" s="47"/>
+      <c r="BF5" s="47"/>
+      <c r="BG5" s="47"/>
+      <c r="BH5" s="47"/>
+      <c r="BI5" s="47"/>
+      <c r="BJ5" s="47"/>
+      <c r="BK5" s="47"/>
+      <c r="BL5" s="47"/>
+      <c r="BM5" s="48"/>
     </row>
     <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
@@ -2480,645 +2483,647 @@
       <c r="C6" s="40">
         <v>44470</v>
       </c>
-      <c r="D6" s="41"/>
+      <c r="D6" s="103" t="s">
+        <v>47</v>
+      </c>
       <c r="E6" s="36"/>
-      <c r="F6" s="42"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="36"/>
       <c r="H6" s="36"/>
-      <c r="I6" s="58" t="str">
+      <c r="I6" s="57" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
         <v>octubre</v>
       </c>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58" t="str">
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57" t="str">
         <f ca="1">IF(TEXT(P7,"mmmm")=I6,"",TEXT(P7,"mmmm"))</f>
         <v/>
       </c>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58" t="str">
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="57" t="str">
         <f ca="1">IF(OR(TEXT(W7,"mmmm")=P6,TEXT(W7,"mmmm")=I6),"",TEXT(W7,"mmmm"))</f>
         <v/>
       </c>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="58"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="58" t="str">
+      <c r="X6" s="57"/>
+      <c r="Y6" s="57"/>
+      <c r="Z6" s="57"/>
+      <c r="AA6" s="57"/>
+      <c r="AB6" s="57"/>
+      <c r="AC6" s="57"/>
+      <c r="AD6" s="57" t="str">
         <f ca="1">IF(OR(TEXT(AD7,"mmmm")=W6,TEXT(AD7,"mmmm")=P6,TEXT(AD7,"mmmm")=I6),"",TEXT(AD7,"mmmm"))</f>
-        <v/>
-      </c>
-      <c r="AE6" s="58"/>
-      <c r="AF6" s="58"/>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="58"/>
-      <c r="AI6" s="58"/>
-      <c r="AJ6" s="58"/>
-      <c r="AK6" s="58" t="str">
+        <v>noviembre</v>
+      </c>
+      <c r="AE6" s="57"/>
+      <c r="AF6" s="57"/>
+      <c r="AG6" s="57"/>
+      <c r="AH6" s="57"/>
+      <c r="AI6" s="57"/>
+      <c r="AJ6" s="57"/>
+      <c r="AK6" s="57" t="str">
         <f ca="1">IF(OR(TEXT(AK7,"mmmm")=AD6,TEXT(AK7,"mmmm")=W6,TEXT(AK7,"mmmm")=P6,TEXT(AK7,"mmmm")=I6),"",TEXT(AK7,"mmmm"))</f>
         <v/>
       </c>
-      <c r="AL6" s="58"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="58"/>
-      <c r="AO6" s="58"/>
-      <c r="AP6" s="58"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="58" t="str">
+      <c r="AL6" s="57"/>
+      <c r="AM6" s="57"/>
+      <c r="AN6" s="57"/>
+      <c r="AO6" s="57"/>
+      <c r="AP6" s="57"/>
+      <c r="AQ6" s="57"/>
+      <c r="AR6" s="57" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>noviembre</v>
-      </c>
-      <c r="AS6" s="58"/>
-      <c r="AT6" s="58"/>
-      <c r="AU6" s="58"/>
-      <c r="AV6" s="58"/>
-      <c r="AW6" s="58"/>
-      <c r="AX6" s="59"/>
-      <c r="AY6" s="59" t="str">
+        <v/>
+      </c>
+      <c r="AS6" s="57"/>
+      <c r="AT6" s="57"/>
+      <c r="AU6" s="57"/>
+      <c r="AV6" s="57"/>
+      <c r="AW6" s="57"/>
+      <c r="AX6" s="58"/>
+      <c r="AY6" s="58" t="str">
         <f ca="1">IF(OR(TEXT(AY7,"mmmm")=AR6,TEXT(AY7,"mmmm")=AK6,TEXT(AY7,"mmmm")=AD6,TEXT(AY7,"mmmm")=W6),"",TEXT(AY7,"mmmm"))</f>
         <v/>
       </c>
-      <c r="AZ6" s="59"/>
-      <c r="BA6" s="59"/>
-      <c r="BB6" s="60"/>
-      <c r="BC6" s="57"/>
-      <c r="BD6" s="57"/>
-      <c r="BE6" s="57"/>
-      <c r="BF6" s="57" t="str">
+      <c r="AZ6" s="58"/>
+      <c r="BA6" s="58"/>
+      <c r="BB6" s="59"/>
+      <c r="BC6" s="56"/>
+      <c r="BD6" s="56"/>
+      <c r="BE6" s="56"/>
+      <c r="BF6" s="56" t="str">
         <f ca="1">IF(OR(TEXT(BF7,"mmmm")=AY6,TEXT(BF7,"mmmm")=AR6,TEXT(BF7,"mmmm")=AK6,TEXT(BF7,"mmmm")=AD6),"",TEXT(BF7,"mmmm"))</f>
-        <v/>
-      </c>
-      <c r="BG6" s="57"/>
-      <c r="BH6" s="57"/>
-      <c r="BI6" s="57"/>
-      <c r="BJ6" s="57"/>
-      <c r="BK6" s="57"/>
-      <c r="BL6" s="57"/>
-      <c r="BM6" s="49"/>
+        <v>diciembre</v>
+      </c>
+      <c r="BG6" s="56"/>
+      <c r="BH6" s="56"/>
+      <c r="BI6" s="56"/>
+      <c r="BJ6" s="56"/>
+      <c r="BK6" s="56"/>
+      <c r="BL6" s="56"/>
+      <c r="BM6" s="48"/>
     </row>
     <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="43">
-        <v>0</v>
+      <c r="C7" s="42">
+        <v>14</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="36"/>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="61">
+      <c r="H7" s="43"/>
+      <c r="I7" s="60">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44470</v>
-      </c>
-      <c r="J7" s="62">
+        <v>44484</v>
+      </c>
+      <c r="J7" s="61">
         <f ca="1">I7+1</f>
-        <v>44471</v>
-      </c>
-      <c r="K7" s="62">
+        <v>44485</v>
+      </c>
+      <c r="K7" s="61">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>44472</v>
-      </c>
-      <c r="L7" s="62">
-        <f t="shared" ca="1" si="0"/>
-        <v>44473</v>
-      </c>
-      <c r="M7" s="62">
-        <f t="shared" ca="1" si="0"/>
-        <v>44474</v>
-      </c>
-      <c r="N7" s="62">
-        <f t="shared" ca="1" si="0"/>
-        <v>44475</v>
-      </c>
-      <c r="O7" s="63">
-        <f t="shared" ca="1" si="0"/>
-        <v>44476</v>
-      </c>
-      <c r="P7" s="62">
-        <f ca="1">O7+1</f>
-        <v>44477</v>
-      </c>
-      <c r="Q7" s="62">
-        <f ca="1">P7+1</f>
-        <v>44478</v>
-      </c>
-      <c r="R7" s="62">
-        <f t="shared" ca="1" si="0"/>
-        <v>44479</v>
-      </c>
-      <c r="S7" s="62">
-        <f t="shared" ca="1" si="0"/>
-        <v>44480</v>
-      </c>
-      <c r="T7" s="62">
-        <f t="shared" ca="1" si="0"/>
-        <v>44481</v>
-      </c>
-      <c r="U7" s="62">
-        <f t="shared" ca="1" si="0"/>
-        <v>44482</v>
-      </c>
-      <c r="V7" s="63">
-        <f t="shared" ca="1" si="0"/>
-        <v>44483</v>
-      </c>
-      <c r="W7" s="62">
-        <f ca="1">V7+1</f>
-        <v>44484</v>
-      </c>
-      <c r="X7" s="62">
-        <f ca="1">W7+1</f>
-        <v>44485</v>
-      </c>
-      <c r="Y7" s="62">
-        <f t="shared" ca="1" si="0"/>
         <v>44486</v>
       </c>
-      <c r="Z7" s="62">
+      <c r="L7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44487</v>
       </c>
-      <c r="AA7" s="62">
+      <c r="M7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44488</v>
       </c>
-      <c r="AB7" s="62">
+      <c r="N7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44489</v>
       </c>
-      <c r="AC7" s="63">
+      <c r="O7" s="62">
         <f t="shared" ca="1" si="0"/>
         <v>44490</v>
       </c>
-      <c r="AD7" s="62">
-        <f ca="1">AC7+1</f>
+      <c r="P7" s="61">
+        <f ca="1">O7+1</f>
         <v>44491</v>
       </c>
-      <c r="AE7" s="62">
-        <f ca="1">AD7+1</f>
+      <c r="Q7" s="61">
+        <f ca="1">P7+1</f>
         <v>44492</v>
       </c>
-      <c r="AF7" s="62">
+      <c r="R7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44493</v>
       </c>
-      <c r="AG7" s="62">
+      <c r="S7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44494</v>
       </c>
-      <c r="AH7" s="62">
+      <c r="T7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44495</v>
       </c>
-      <c r="AI7" s="62">
+      <c r="U7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44496</v>
       </c>
-      <c r="AJ7" s="63">
+      <c r="V7" s="62">
         <f t="shared" ca="1" si="0"/>
         <v>44497</v>
       </c>
-      <c r="AK7" s="62">
-        <f ca="1">AJ7+1</f>
+      <c r="W7" s="61">
+        <f ca="1">V7+1</f>
         <v>44498</v>
       </c>
-      <c r="AL7" s="62">
-        <f ca="1">AK7+1</f>
+      <c r="X7" s="61">
+        <f ca="1">W7+1</f>
         <v>44499</v>
       </c>
-      <c r="AM7" s="62">
-        <f t="shared" ref="AM7" ca="1" si="1">AL7+1</f>
+      <c r="Y7" s="61">
+        <f t="shared" ca="1" si="0"/>
         <v>44500</v>
       </c>
-      <c r="AN7" s="62">
-        <f t="shared" ref="AN7" ca="1" si="2">AM7+1</f>
+      <c r="Z7" s="61">
+        <f t="shared" ca="1" si="0"/>
         <v>44501</v>
       </c>
-      <c r="AO7" s="63">
-        <f t="shared" ref="AO7:AQ7" ca="1" si="3">AN7+1</f>
+      <c r="AA7" s="61">
+        <f t="shared" ca="1" si="0"/>
         <v>44502</v>
       </c>
-      <c r="AP7" s="62">
-        <f t="shared" ca="1" si="3"/>
+      <c r="AB7" s="61">
+        <f t="shared" ca="1" si="0"/>
         <v>44503</v>
       </c>
-      <c r="AQ7" s="62">
-        <f t="shared" ca="1" si="3"/>
+      <c r="AC7" s="62">
+        <f t="shared" ca="1" si="0"/>
         <v>44504</v>
       </c>
-      <c r="AR7" s="62">
-        <f t="shared" ref="AR7" ca="1" si="4">AQ7+1</f>
+      <c r="AD7" s="61">
+        <f ca="1">AC7+1</f>
         <v>44505</v>
       </c>
-      <c r="AS7" s="62">
-        <f ca="1">AR7+1</f>
+      <c r="AE7" s="61">
+        <f ca="1">AD7+1</f>
         <v>44506</v>
       </c>
-      <c r="AT7" s="62">
+      <c r="AF7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44507</v>
       </c>
-      <c r="AU7" s="62">
+      <c r="AG7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44508</v>
       </c>
-      <c r="AV7" s="62">
+      <c r="AH7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44509</v>
       </c>
-      <c r="AW7" s="62">
+      <c r="AI7" s="61">
         <f t="shared" ca="1" si="0"/>
         <v>44510</v>
       </c>
-      <c r="AX7" s="63">
+      <c r="AJ7" s="62">
         <f t="shared" ca="1" si="0"/>
         <v>44511</v>
       </c>
-      <c r="AY7" s="62">
+      <c r="AK7" s="61">
+        <f ca="1">AJ7+1</f>
+        <v>44512</v>
+      </c>
+      <c r="AL7" s="61">
+        <f ca="1">AK7+1</f>
+        <v>44513</v>
+      </c>
+      <c r="AM7" s="61">
+        <f t="shared" ref="AM7" ca="1" si="1">AL7+1</f>
+        <v>44514</v>
+      </c>
+      <c r="AN7" s="61">
+        <f t="shared" ref="AN7" ca="1" si="2">AM7+1</f>
+        <v>44515</v>
+      </c>
+      <c r="AO7" s="62">
+        <f t="shared" ref="AO7:AQ7" ca="1" si="3">AN7+1</f>
+        <v>44516</v>
+      </c>
+      <c r="AP7" s="61">
+        <f t="shared" ca="1" si="3"/>
+        <v>44517</v>
+      </c>
+      <c r="AQ7" s="61">
+        <f t="shared" ca="1" si="3"/>
+        <v>44518</v>
+      </c>
+      <c r="AR7" s="61">
+        <f t="shared" ref="AR7" ca="1" si="4">AQ7+1</f>
+        <v>44519</v>
+      </c>
+      <c r="AS7" s="61">
+        <f ca="1">AR7+1</f>
+        <v>44520</v>
+      </c>
+      <c r="AT7" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>44521</v>
+      </c>
+      <c r="AU7" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>44522</v>
+      </c>
+      <c r="AV7" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>44523</v>
+      </c>
+      <c r="AW7" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>44524</v>
+      </c>
+      <c r="AX7" s="62">
+        <f t="shared" ca="1" si="0"/>
+        <v>44525</v>
+      </c>
+      <c r="AY7" s="61">
         <f ca="1">AX7+1</f>
-        <v>44512</v>
-      </c>
-      <c r="AZ7" s="62">
+        <v>44526</v>
+      </c>
+      <c r="AZ7" s="61">
         <f ca="1">AY7+1</f>
-        <v>44513</v>
-      </c>
-      <c r="BA7" s="62">
+        <v>44527</v>
+      </c>
+      <c r="BA7" s="61">
         <f t="shared" ref="BA7:BE7" ca="1" si="5">AZ7+1</f>
-        <v>44514</v>
-      </c>
-      <c r="BB7" s="62">
+        <v>44528</v>
+      </c>
+      <c r="BB7" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>44515</v>
-      </c>
-      <c r="BC7" s="62">
+        <v>44529</v>
+      </c>
+      <c r="BC7" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>44516</v>
-      </c>
-      <c r="BD7" s="62">
+        <v>44530</v>
+      </c>
+      <c r="BD7" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>44517</v>
-      </c>
-      <c r="BE7" s="63">
+        <v>44531</v>
+      </c>
+      <c r="BE7" s="62">
         <f t="shared" ca="1" si="5"/>
-        <v>44518</v>
-      </c>
-      <c r="BF7" s="62">
+        <v>44532</v>
+      </c>
+      <c r="BF7" s="61">
         <f ca="1">BE7+1</f>
-        <v>44519</v>
-      </c>
-      <c r="BG7" s="62">
+        <v>44533</v>
+      </c>
+      <c r="BG7" s="61">
         <f ca="1">BF7+1</f>
-        <v>44520</v>
-      </c>
-      <c r="BH7" s="62">
+        <v>44534</v>
+      </c>
+      <c r="BH7" s="61">
         <f t="shared" ref="BH7:BL7" ca="1" si="6">BG7+1</f>
-        <v>44521</v>
-      </c>
-      <c r="BI7" s="62">
+        <v>44535</v>
+      </c>
+      <c r="BI7" s="61">
         <f t="shared" ca="1" si="6"/>
-        <v>44522</v>
-      </c>
-      <c r="BJ7" s="62">
+        <v>44536</v>
+      </c>
+      <c r="BJ7" s="61">
         <f t="shared" ca="1" si="6"/>
-        <v>44523</v>
-      </c>
-      <c r="BK7" s="62">
+        <v>44537</v>
+      </c>
+      <c r="BK7" s="61">
         <f t="shared" ca="1" si="6"/>
-        <v>44524</v>
-      </c>
-      <c r="BL7" s="63">
+        <v>44538</v>
+      </c>
+      <c r="BL7" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>44525</v>
-      </c>
-      <c r="BM7" s="49"/>
+        <v>44539</v>
+      </c>
+      <c r="BM7" s="48"/>
     </row>
     <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
-      <c r="U8" s="65"/>
-      <c r="V8" s="67"/>
-      <c r="W8" s="65"/>
-      <c r="X8" s="65"/>
-      <c r="Y8" s="65"/>
-      <c r="Z8" s="65"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="65"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="65"/>
-      <c r="AH8" s="65"/>
-      <c r="AI8" s="65"/>
-      <c r="AJ8" s="67"/>
-      <c r="AK8" s="65"/>
-      <c r="AL8" s="65"/>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="65"/>
-      <c r="AO8" s="67"/>
-      <c r="AP8" s="65"/>
-      <c r="AQ8" s="65"/>
-      <c r="AR8" s="65"/>
-      <c r="AS8" s="65"/>
-      <c r="AT8" s="65"/>
-      <c r="AU8" s="65"/>
-      <c r="AV8" s="65"/>
-      <c r="AW8" s="65"/>
-      <c r="AX8" s="67"/>
-      <c r="AY8" s="65"/>
-      <c r="AZ8" s="65"/>
-      <c r="BA8" s="65"/>
-      <c r="BB8" s="65"/>
-      <c r="BC8" s="65"/>
-      <c r="BD8" s="65"/>
-      <c r="BE8" s="67"/>
-      <c r="BF8" s="65"/>
-      <c r="BG8" s="65"/>
-      <c r="BH8" s="65"/>
-      <c r="BI8" s="65"/>
-      <c r="BJ8" s="65"/>
-      <c r="BK8" s="65"/>
-      <c r="BL8" s="68"/>
-      <c r="BM8" s="49"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="64"/>
+      <c r="S8" s="64"/>
+      <c r="T8" s="64"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="66"/>
+      <c r="W8" s="64"/>
+      <c r="X8" s="64"/>
+      <c r="Y8" s="64"/>
+      <c r="Z8" s="64"/>
+      <c r="AA8" s="64"/>
+      <c r="AB8" s="64"/>
+      <c r="AC8" s="66"/>
+      <c r="AD8" s="64"/>
+      <c r="AE8" s="64"/>
+      <c r="AF8" s="64"/>
+      <c r="AG8" s="64"/>
+      <c r="AH8" s="64"/>
+      <c r="AI8" s="64"/>
+      <c r="AJ8" s="66"/>
+      <c r="AK8" s="64"/>
+      <c r="AL8" s="64"/>
+      <c r="AM8" s="64"/>
+      <c r="AN8" s="64"/>
+      <c r="AO8" s="66"/>
+      <c r="AP8" s="64"/>
+      <c r="AQ8" s="64"/>
+      <c r="AR8" s="64"/>
+      <c r="AS8" s="64"/>
+      <c r="AT8" s="64"/>
+      <c r="AU8" s="64"/>
+      <c r="AV8" s="64"/>
+      <c r="AW8" s="64"/>
+      <c r="AX8" s="66"/>
+      <c r="AY8" s="64"/>
+      <c r="AZ8" s="64"/>
+      <c r="BA8" s="64"/>
+      <c r="BB8" s="64"/>
+      <c r="BC8" s="64"/>
+      <c r="BD8" s="64"/>
+      <c r="BE8" s="66"/>
+      <c r="BF8" s="64"/>
+      <c r="BG8" s="64"/>
+      <c r="BH8" s="64"/>
+      <c r="BI8" s="64"/>
+      <c r="BJ8" s="64"/>
+      <c r="BK8" s="64"/>
+      <c r="BL8" s="67"/>
+      <c r="BM8" s="48"/>
     </row>
     <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="78" t="s">
+      <c r="D9" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="78" t="s">
+      <c r="F9" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="78" t="s">
+      <c r="G9" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="69" t="str">
+      <c r="H9" s="54"/>
+      <c r="I9" s="68" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="7">LEFT(TEXT(I7,"ddd"),1)</f>
         <v>v</v>
       </c>
-      <c r="J9" s="69" t="str">
+      <c r="J9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="K9" s="69" t="str">
+      <c r="K9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="L9" s="69" t="str">
+      <c r="L9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="M9" s="69" t="str">
+      <c r="M9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="N9" s="69" t="str">
+      <c r="N9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="O9" s="69" t="str">
+      <c r="O9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="P9" s="69" t="str">
+      <c r="P9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>v</v>
       </c>
-      <c r="Q9" s="69" t="str">
+      <c r="Q9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="R9" s="69" t="str">
+      <c r="R9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="S9" s="69" t="str">
+      <c r="S9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="T9" s="69" t="str">
+      <c r="T9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="U9" s="69" t="str">
+      <c r="U9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="V9" s="69" t="str">
+      <c r="V9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="W9" s="69" t="str">
+      <c r="W9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>v</v>
       </c>
-      <c r="X9" s="69" t="str">
+      <c r="X9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="Y9" s="69" t="str">
+      <c r="Y9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="Z9" s="69" t="str">
+      <c r="Z9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="AA9" s="69" t="str">
+      <c r="AA9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AB9" s="69" t="str">
+      <c r="AB9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AC9" s="69" t="str">
+      <c r="AC9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="AD9" s="69" t="str">
+      <c r="AD9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>v</v>
       </c>
-      <c r="AE9" s="69" t="str">
+      <c r="AE9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="AF9" s="69" t="str">
+      <c r="AF9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="AG9" s="69" t="str">
+      <c r="AG9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="AH9" s="69" t="str">
+      <c r="AH9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AI9" s="69" t="str">
+      <c r="AI9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AJ9" s="69" t="str">
+      <c r="AJ9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="AK9" s="69" t="str">
+      <c r="AK9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>v</v>
       </c>
-      <c r="AL9" s="69" t="str">
+      <c r="AL9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="AM9" s="69" t="str">
+      <c r="AM9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="AN9" s="69" t="str">
+      <c r="AN9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="AO9" s="69" t="str">
+      <c r="AO9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AP9" s="69" t="str">
+      <c r="AP9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AQ9" s="69" t="str">
+      <c r="AQ9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="AR9" s="69" t="str">
+      <c r="AR9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>v</v>
       </c>
-      <c r="AS9" s="69" t="str">
+      <c r="AS9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="AT9" s="69" t="str">
+      <c r="AT9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="AU9" s="69" t="str">
+      <c r="AU9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="AV9" s="69" t="str">
+      <c r="AV9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AW9" s="69" t="str">
+      <c r="AW9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="AX9" s="69" t="str">
+      <c r="AX9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="AY9" s="69" t="str">
+      <c r="AY9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>v</v>
       </c>
-      <c r="AZ9" s="69" t="str">
+      <c r="AZ9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="BA9" s="69" t="str">
+      <c r="BA9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="BB9" s="69" t="str">
+      <c r="BB9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="BC9" s="69" t="str">
+      <c r="BC9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="BD9" s="69" t="str">
+      <c r="BD9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="BE9" s="69" t="str">
+      <c r="BE9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="BF9" s="69" t="str">
+      <c r="BF9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>v</v>
       </c>
-      <c r="BG9" s="69" t="str">
+      <c r="BG9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>s</v>
       </c>
-      <c r="BH9" s="69" t="str">
+      <c r="BH9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>d</v>
       </c>
-      <c r="BI9" s="69" t="str">
+      <c r="BI9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>l</v>
       </c>
-      <c r="BJ9" s="69" t="str">
+      <c r="BJ9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="BK9" s="69" t="str">
+      <c r="BK9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>m</v>
       </c>
-      <c r="BL9" s="69" t="str">
+      <c r="BL9" s="68" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>j</v>
       </c>
-      <c r="BM9" s="49"/>
+      <c r="BM9" s="48"/>
     </row>
     <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18"/>
@@ -3127,7 +3132,7 @@
       <c r="E10" s="15"/>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="49"/>
+      <c r="H10" s="48"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
@@ -3158,11 +3163,11 @@
       <c r="AJ10" s="21"/>
       <c r="AK10" s="21"/>
       <c r="AL10" s="21"/>
-      <c r="AM10" s="90"/>
-      <c r="AN10" s="90"/>
-      <c r="AO10" s="90"/>
-      <c r="AP10" s="90"/>
-      <c r="AQ10" s="90"/>
+      <c r="AM10" s="80"/>
+      <c r="AN10" s="80"/>
+      <c r="AO10" s="80"/>
+      <c r="AP10" s="80"/>
+      <c r="AQ10" s="80"/>
       <c r="AR10" s="21"/>
       <c r="AS10" s="21"/>
       <c r="AT10" s="21"/>
@@ -3184,11 +3189,11 @@
       <c r="BJ10" s="21"/>
       <c r="BK10" s="21"/>
       <c r="BL10" s="21"/>
-      <c r="BM10" s="49"/>
+      <c r="BM10" s="48"/>
     </row>
     <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="78" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="23"/>
@@ -3196,7 +3201,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="25"/>
       <c r="G11" s="26"/>
-      <c r="H11" s="53"/>
+      <c r="H11" s="52"/>
       <c r="I11" s="20" t="str">
         <f t="shared" ref="I11:X29" ca="1" si="8">IF(AND($C11="Goal",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
@@ -3436,7 +3441,7 @@
         <v>23</v>
       </c>
       <c r="E12" s="24">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F12" s="25">
         <v>44470</v>
@@ -3444,7 +3449,7 @@
       <c r="G12" s="26">
         <v>4</v>
       </c>
-      <c r="H12" s="53"/>
+      <c r="H12" s="52"/>
       <c r="I12" s="20" t="str">
         <f ca="1">IF(AND($C12="Goal",I$7&gt;=$F12,I$7&lt;=$F12+$G12-1),2,IF(AND($C12="Milestone",I$7&gt;=$F12,I$7&lt;=$F12+$G12-1),1,""))</f>
         <v/>
@@ -3481,7 +3486,7 @@
         <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
-      <c r="R12" s="56" t="str">
+      <c r="R12" s="55" t="str">
         <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
@@ -3673,25 +3678,25 @@
     </row>
     <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="98" t="s">
+      <c r="C13" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="99">
+      <c r="E13" s="89">
         <v>0</v>
       </c>
-      <c r="F13" s="100">
+      <c r="F13" s="90">
         <v>44473</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="91">
         <v>3</v>
       </c>
-      <c r="H13" s="53"/>
+      <c r="H13" s="52"/>
       <c r="I13" s="20" t="str">
         <f t="shared" ref="I13:X29" ca="1" si="13">IF(AND($C13="Goal",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),2,IF(AND($C13="Milestone",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),1,""))</f>
         <v/>
@@ -3938,7 +3943,7 @@
       <c r="G14" s="26">
         <v>1</v>
       </c>
-      <c r="H14" s="53"/>
+      <c r="H14" s="52"/>
       <c r="I14" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -3959,9 +3964,9 @@
         <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
-      <c r="N14" s="20">
-        <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+      <c r="N14" s="20" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v/>
       </c>
       <c r="O14" s="20" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4185,7 +4190,7 @@
       <c r="G15" s="26">
         <v>7</v>
       </c>
-      <c r="H15" s="53"/>
+      <c r="H15" s="52"/>
       <c r="I15" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -4414,25 +4419,25 @@
     </row>
     <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="92" t="s">
+      <c r="D16" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="93">
+      <c r="E16" s="83">
         <v>0</v>
       </c>
-      <c r="F16" s="94">
+      <c r="F16" s="84">
         <v>44482</v>
       </c>
-      <c r="G16" s="95">
+      <c r="G16" s="85">
         <v>1</v>
       </c>
-      <c r="H16" s="53"/>
+      <c r="H16" s="52"/>
       <c r="I16" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -4481,9 +4486,9 @@
         <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
-      <c r="U16" s="20">
-        <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+      <c r="U16" s="20" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v/>
       </c>
       <c r="V16" s="20" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -4679,7 +4684,7 @@
       <c r="G17" s="26">
         <v>5</v>
       </c>
-      <c r="H17" s="53"/>
+      <c r="H17" s="52"/>
       <c r="I17" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -4926,7 +4931,7 @@
       <c r="G18" s="26">
         <v>14</v>
       </c>
-      <c r="H18" s="53"/>
+      <c r="H18" s="52"/>
       <c r="I18" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -4939,117 +4944,117 @@
         <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="L18" s="20" t="str">
+      <c r="L18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="M18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="M18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="N18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="N18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="O18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="O18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="P18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="P18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="Q18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="R18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="R18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="S18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="S18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="T18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="T18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="U18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="U18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="V18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="V18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="W18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="W18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="X18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="X18" s="20">
         <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="Y18" s="20" t="str">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="20">
         <f t="shared" ref="Y18:BD24" ca="1" si="15">IF(AND($C18="Goal",Y$7&gt;=$F18,Y$7&lt;=$F18+$G18-1),2,IF(AND($C18="Milestone",Y$7&gt;=$F18,Y$7&lt;=$F18+$G18-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="Z18" s="20">
-        <f t="shared" ca="1" si="15"/>
         <v>2</v>
       </c>
-      <c r="AA18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AB18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AC18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AD18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AE18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AF18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AG18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AH18" s="96">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AI18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AJ18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AK18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AL18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AM18" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>2</v>
+      <c r="Z18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AA18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AB18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AC18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AD18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AE18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AF18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AG18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AH18" s="86" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AI18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AJ18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AK18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AL18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
+      </c>
+      <c r="AM18" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
       </c>
       <c r="AN18" s="20" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -5173,229 +5178,229 @@
       <c r="G19" s="26">
         <v>2</v>
       </c>
-      <c r="H19" s="53"/>
+      <c r="H19" s="52"/>
       <c r="I19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ref="I19:AN19" ca="1" si="16">IF(AND($C19="Goal",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",I$7&gt;=$F19,I$7&lt;=$F19+$G19-1),1,""))</f>
         <v/>
       </c>
       <c r="J19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",J$7&gt;=$F19,J$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",J$7&gt;=$F19,J$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="K19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",K$7&gt;=$F19,K$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",K$7&gt;=$F19,K$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="L19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",L$7&gt;=$F19,L$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",L$7&gt;=$F19,L$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="M19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",M$7&gt;=$F19,M$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",M$7&gt;=$F19,M$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="N19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",N$7&gt;=$F19,N$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",N$7&gt;=$F19,N$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="O19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",O$7&gt;=$F19,O$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",O$7&gt;=$F19,O$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="P19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",P$7&gt;=$F19,P$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",P$7&gt;=$F19,P$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="Q19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",Q$7&gt;=$F19,Q$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",Q$7&gt;=$F19,Q$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="R19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",R$7&gt;=$F19,R$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",R$7&gt;=$F19,R$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="S19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",S$7&gt;=$F19,S$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",S$7&gt;=$F19,S$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="T19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",T$7&gt;=$F19,T$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",T$7&gt;=$F19,T$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="U19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",U$7&gt;=$F19,U$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",U$7&gt;=$F19,U$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="V19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",V$7&gt;=$F19,V$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",V$7&gt;=$F19,V$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="W19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",W$7&gt;=$F19,W$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",W$7&gt;=$F19,W$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="X19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",X$7&gt;=$F19,X$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",X$7&gt;=$F19,X$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="Y19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",Y$7&gt;=$F19,Y$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",Y$7&gt;=$F19,Y$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="Z19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",Z$7&gt;=$F19,Z$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",Z$7&gt;=$F19,Z$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AA19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AA$7&gt;=$F19,AA$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AA$7&gt;=$F19,AA$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AB19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AB$7&gt;=$F19,AB$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AB$7&gt;=$F19,AB$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AC19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AC$7&gt;=$F19,AC$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AC$7&gt;=$F19,AC$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AD19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AD$7&gt;=$F19,AD$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AD$7&gt;=$F19,AD$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AE19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AE$7&gt;=$F19,AE$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AE$7&gt;=$F19,AE$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AF19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AF$7&gt;=$F19,AF$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AF$7&gt;=$F19,AF$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AG19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AG$7&gt;=$F19,AG$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AG$7&gt;=$F19,AG$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AH19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AH$7&gt;=$F19,AH$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AH$7&gt;=$F19,AH$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AI19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AI$7&gt;=$F19,AI$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AI$7&gt;=$F19,AI$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AJ19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AJ$7&gt;=$F19,AJ$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AJ$7&gt;=$F19,AJ$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AK19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AK$7&gt;=$F19,AK$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AK$7&gt;=$F19,AK$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AL19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AL$7&gt;=$F19,AL$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AL$7&gt;=$F19,AL$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AM19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AM$7&gt;=$F19,AM$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AM$7&gt;=$F19,AM$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AN19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AN$7&gt;=$F19,AN$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AN$7&gt;=$F19,AN$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AO19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AO$7&gt;=$F19,AO$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AO$7&gt;=$F19,AO$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AP19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AP$7&gt;=$F19,AP$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AP$7&gt;=$F19,AP$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AQ19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AQ$7&gt;=$F19,AQ$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AQ$7&gt;=$F19,AQ$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AR19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AR$7&gt;=$F19,AR$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AR$7&gt;=$F19,AR$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AS19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AS$7&gt;=$F19,AS$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AS$7&gt;=$F19,AS$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AT19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AT$7&gt;=$F19,AT$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AT$7&gt;=$F19,AT$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AU19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AU$7&gt;=$F19,AU$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AU$7&gt;=$F19,AU$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AV19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AV$7&gt;=$F19,AV$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AV$7&gt;=$F19,AV$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AW19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AW$7&gt;=$F19,AW$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AW$7&gt;=$F19,AW$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AX19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AX$7&gt;=$F19,AX$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AX$7&gt;=$F19,AX$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AY19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AY$7&gt;=$F19,AY$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AY$7&gt;=$F19,AY$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AZ19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",AZ$7&gt;=$F19,AZ$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",AZ$7&gt;=$F19,AZ$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BA19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BA$7&gt;=$F19,BA$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BA$7&gt;=$F19,BA$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BB19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BB$7&gt;=$F19,BB$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BB$7&gt;=$F19,BB$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BC19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BC$7&gt;=$F19,BC$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BC$7&gt;=$F19,BC$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BD19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BD$7&gt;=$F19,BD$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BD$7&gt;=$F19,BD$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BE19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BE$7&gt;=$F19,BE$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BE$7&gt;=$F19,BE$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BF19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BF$7&gt;=$F19,BF$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BF$7&gt;=$F19,BF$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BG19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BG$7&gt;=$F19,BG$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BG$7&gt;=$F19,BG$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BH19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BH$7&gt;=$F19,BH$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BH$7&gt;=$F19,BH$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BI19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BI$7&gt;=$F19,BI$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BI$7&gt;=$F19,BI$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BJ19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BJ$7&gt;=$F19,BJ$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BJ$7&gt;=$F19,BJ$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BK19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BK$7&gt;=$F19,BK$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BK$7&gt;=$F19,BK$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BL19" s="20" t="str">
-        <f ca="1">IF(AND($C19="Goal",BL$7&gt;=$F19,BL$7&lt;=$F19+$G19-1),2,IF(AND($C19="Milestone",BL$7&gt;=$F19,BL$7&lt;=$F19+$G19-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BM19" s="19"/>
@@ -5420,248 +5425,248 @@
       <c r="G20" s="26">
         <v>4</v>
       </c>
-      <c r="H20" s="53"/>
+      <c r="H20" s="52"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",J$7&gt;=$F20,J$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",J$7&gt;=$F20,J$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ref="J20:S21" ca="1" si="17">IF(AND($C20="Goal",J$7&gt;=$F20,J$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",J$7&gt;=$F20,J$7&lt;=$F20+$G20-1),1,""))</f>
         <v/>
       </c>
       <c r="K20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",K$7&gt;=$F20,K$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",K$7&gt;=$F20,K$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="L20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",L$7&gt;=$F20,L$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",L$7&gt;=$F20,L$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="M20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",M$7&gt;=$F20,M$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",M$7&gt;=$F20,M$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="N20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",N$7&gt;=$F20,N$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",N$7&gt;=$F20,N$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="O20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",O$7&gt;=$F20,O$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",O$7&gt;=$F20,O$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="P20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",P$7&gt;=$F20,P$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",P$7&gt;=$F20,P$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="Q20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",Q$7&gt;=$F20,Q$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",Q$7&gt;=$F20,Q$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="R20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",R$7&gt;=$F20,R$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",R$7&gt;=$F20,R$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="S20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",S$7&gt;=$F20,S$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",S$7&gt;=$F20,S$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="T20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",T$7&gt;=$F20,T$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",T$7&gt;=$F20,T$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ref="T20:AC21" ca="1" si="18">IF(AND($C20="Goal",T$7&gt;=$F20,T$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",T$7&gt;=$F20,T$7&lt;=$F20+$G20-1),1,""))</f>
         <v/>
       </c>
       <c r="U20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",U$7&gt;=$F20,U$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",U$7&gt;=$F20,U$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="V20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",V$7&gt;=$F20,V$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",V$7&gt;=$F20,V$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="W20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",W$7&gt;=$F20,W$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",W$7&gt;=$F20,W$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="X20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",X$7&gt;=$F20,X$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",X$7&gt;=$F20,X$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="Y20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",Y$7&gt;=$F20,Y$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",Y$7&gt;=$F20,Y$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="Z20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",Z$7&gt;=$F20,Z$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",Z$7&gt;=$F20,Z$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AA20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AA$7&gt;=$F20,AA$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AA$7&gt;=$F20,AA$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AB20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AB$7&gt;=$F20,AB$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AB$7&gt;=$F20,AB$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AC20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AC$7&gt;=$F20,AC$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AC$7&gt;=$F20,AC$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AD20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AD$7&gt;=$F20,AD$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AD$7&gt;=$F20,AD$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ref="AD20:AM21" ca="1" si="19">IF(AND($C20="Goal",AD$7&gt;=$F20,AD$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AD$7&gt;=$F20,AD$7&lt;=$F20+$G20-1),1,""))</f>
         <v/>
       </c>
       <c r="AE20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AE$7&gt;=$F20,AE$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AE$7&gt;=$F20,AE$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AF20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AF$7&gt;=$F20,AF$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AF$7&gt;=$F20,AF$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AG20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AG$7&gt;=$F20,AG$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AG$7&gt;=$F20,AG$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AH20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AH$7&gt;=$F20,AH$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AH$7&gt;=$F20,AH$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AI20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AI$7&gt;=$F20,AI$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AI$7&gt;=$F20,AI$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AJ20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AJ$7&gt;=$F20,AJ$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AJ$7&gt;=$F20,AJ$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AK20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AK$7&gt;=$F20,AK$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AK$7&gt;=$F20,AK$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AL20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AL$7&gt;=$F20,AL$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AL$7&gt;=$F20,AL$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AM20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AM$7&gt;=$F20,AM$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AM$7&gt;=$F20,AM$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AN20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AN$7&gt;=$F20,AN$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AN$7&gt;=$F20,AN$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ref="AN20:AW21" ca="1" si="20">IF(AND($C20="Goal",AN$7&gt;=$F20,AN$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AN$7&gt;=$F20,AN$7&lt;=$F20+$G20-1),1,""))</f>
         <v/>
       </c>
       <c r="AO20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AO$7&gt;=$F20,AO$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AO$7&gt;=$F20,AO$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AP20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AP$7&gt;=$F20,AP$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AP$7&gt;=$F20,AP$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AQ20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AQ$7&gt;=$F20,AQ$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AQ$7&gt;=$F20,AQ$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AR20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AR$7&gt;=$F20,AR$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AR$7&gt;=$F20,AR$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AS20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AS$7&gt;=$F20,AS$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AS$7&gt;=$F20,AS$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AT20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AT$7&gt;=$F20,AT$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AT$7&gt;=$F20,AT$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AU20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AU$7&gt;=$F20,AU$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AU$7&gt;=$F20,AU$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AV20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AV$7&gt;=$F20,AV$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AV$7&gt;=$F20,AV$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AW20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AW$7&gt;=$F20,AW$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AW$7&gt;=$F20,AW$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AX20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AX$7&gt;=$F20,AX$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AX$7&gt;=$F20,AX$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AY20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AY$7&gt;=$F20,AY$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AY$7&gt;=$F20,AY$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AZ20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",AZ$7&gt;=$F20,AZ$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",AZ$7&gt;=$F20,AZ$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BA20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BA$7&gt;=$F20,BA$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BA$7&gt;=$F20,BA$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BB20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BB$7&gt;=$F20,BB$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BB$7&gt;=$F20,BB$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BC20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BC$7&gt;=$F20,BC$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BC$7&gt;=$F20,BC$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BD20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BD$7&gt;=$F20,BD$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BD$7&gt;=$F20,BD$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BE20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BE$7&gt;=$F20,BE$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BE$7&gt;=$F20,BE$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BF20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BF$7&gt;=$F20,BF$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BF$7&gt;=$F20,BF$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BG20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BG$7&gt;=$F20,BG$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BG$7&gt;=$F20,BG$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BH20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BH$7&gt;=$F20,BH$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BH$7&gt;=$F20,BH$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BI20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BI$7&gt;=$F20,BI$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BI$7&gt;=$F20,BI$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BJ20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BJ$7&gt;=$F20,BJ$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BJ$7&gt;=$F20,BJ$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BK20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BK$7&gt;=$F20,BK$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BK$7&gt;=$F20,BK$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BL20" s="20" t="str">
-        <f ca="1">IF(AND($C20="Goal",BL$7&gt;=$F20,BL$7&lt;=$F20+$G20-1),2,IF(AND($C20="Milestone",BL$7&gt;=$F20,BL$7&lt;=$F20+$G20-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BM20" s="19"/>
     </row>
     <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="92" t="s">
+      <c r="D21" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="93">
+      <c r="E21" s="83">
         <v>0</v>
       </c>
-      <c r="F21" s="94">
+      <c r="F21" s="84">
         <v>44501</v>
       </c>
-      <c r="G21" s="95">
+      <c r="G21" s="85">
         <v>7</v>
       </c>
       <c r="H21" s="12"/>
@@ -5670,230 +5675,230 @@
         <v/>
       </c>
       <c r="J21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",J$7&gt;=$F21,J$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",J$7&gt;=$F21,J$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="K21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",K$7&gt;=$F21,K$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",K$7&gt;=$F21,K$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="L21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",L$7&gt;=$F21,L$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",L$7&gt;=$F21,L$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="M21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",M$7&gt;=$F21,M$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",M$7&gt;=$F21,M$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="N21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",N$7&gt;=$F21,N$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",N$7&gt;=$F21,N$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="O21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",O$7&gt;=$F21,O$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",O$7&gt;=$F21,O$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="P21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",P$7&gt;=$F21,P$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",P$7&gt;=$F21,P$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="Q21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",Q$7&gt;=$F21,Q$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",Q$7&gt;=$F21,Q$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="R21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",R$7&gt;=$F21,R$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",R$7&gt;=$F21,R$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="S21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",S$7&gt;=$F21,S$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",S$7&gt;=$F21,S$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="T21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",T$7&gt;=$F21,T$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",T$7&gt;=$F21,T$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="U21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",U$7&gt;=$F21,U$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",U$7&gt;=$F21,U$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="V21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",V$7&gt;=$F21,V$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",V$7&gt;=$F21,V$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="W21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",W$7&gt;=$F21,W$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",W$7&gt;=$F21,W$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="X21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",X$7&gt;=$F21,X$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",X$7&gt;=$F21,X$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="Y21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",Y$7&gt;=$F21,Y$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",Y$7&gt;=$F21,Y$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="Z21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",Z$7&gt;=$F21,Z$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",Z$7&gt;=$F21,Z$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AA21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AA$7&gt;=$F21,AA$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AA$7&gt;=$F21,AA$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AB21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AB$7&gt;=$F21,AB$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AB$7&gt;=$F21,AB$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AC21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AC$7&gt;=$F21,AC$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AC$7&gt;=$F21,AC$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="18"/>
         <v/>
       </c>
       <c r="AD21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AD$7&gt;=$F21,AD$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AD$7&gt;=$F21,AD$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AE21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AE$7&gt;=$F21,AE$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AE$7&gt;=$F21,AE$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AF21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AF$7&gt;=$F21,AF$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AF$7&gt;=$F21,AF$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AG21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AG$7&gt;=$F21,AG$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AG$7&gt;=$F21,AG$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AH21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AH$7&gt;=$F21,AH$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AH$7&gt;=$F21,AH$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AI21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AI$7&gt;=$F21,AI$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AI$7&gt;=$F21,AI$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AJ21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AJ$7&gt;=$F21,AJ$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AJ$7&gt;=$F21,AJ$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AK21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AK$7&gt;=$F21,AK$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AK$7&gt;=$F21,AK$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AL21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AL$7&gt;=$F21,AL$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AL$7&gt;=$F21,AL$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AM21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AM$7&gt;=$F21,AM$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AM$7&gt;=$F21,AM$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="19"/>
         <v/>
       </c>
       <c r="AN21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AN$7&gt;=$F21,AN$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AN$7&gt;=$F21,AN$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AO21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AO$7&gt;=$F21,AO$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AO$7&gt;=$F21,AO$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AP21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AP$7&gt;=$F21,AP$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AP$7&gt;=$F21,AP$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AQ21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AQ$7&gt;=$F21,AQ$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AQ$7&gt;=$F21,AQ$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AR21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AR$7&gt;=$F21,AR$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AR$7&gt;=$F21,AR$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AS21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AS$7&gt;=$F21,AS$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AS$7&gt;=$F21,AS$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AT21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AT$7&gt;=$F21,AT$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AT$7&gt;=$F21,AT$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AU21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AU$7&gt;=$F21,AU$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AU$7&gt;=$F21,AU$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AV21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AV$7&gt;=$F21,AV$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AV$7&gt;=$F21,AV$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AW21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AW$7&gt;=$F21,AW$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AW$7&gt;=$F21,AW$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="20"/>
         <v/>
       </c>
       <c r="AX21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AX$7&gt;=$F21,AX$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AX$7&gt;=$F21,AX$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AY21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AY$7&gt;=$F21,AY$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AY$7&gt;=$F21,AY$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AZ21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",AZ$7&gt;=$F21,AZ$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",AZ$7&gt;=$F21,AZ$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BA21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BA$7&gt;=$F21,BA$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BA$7&gt;=$F21,BA$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BB21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BB$7&gt;=$F21,BB$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BB$7&gt;=$F21,BB$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BC21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BC$7&gt;=$F21,BC$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BC$7&gt;=$F21,BC$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BD21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BD$7&gt;=$F21,BD$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BD$7&gt;=$F21,BD$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="BE21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BE$7&gt;=$F21,BE$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BE$7&gt;=$F21,BE$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BF21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BF$7&gt;=$F21,BF$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BF$7&gt;=$F21,BF$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BG21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BG$7&gt;=$F21,BG$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BG$7&gt;=$F21,BG$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BH21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BH$7&gt;=$F21,BH$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BH$7&gt;=$F21,BH$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BI21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BI$7&gt;=$F21,BI$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BI$7&gt;=$F21,BI$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BJ21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BJ$7&gt;=$F21,BJ$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BJ$7&gt;=$F21,BJ$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BK21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BK$7&gt;=$F21,BK$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BK$7&gt;=$F21,BK$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BL21" s="20" t="str">
-        <f ca="1">IF(AND($C21="Goal",BL$7&gt;=$F21,BL$7&lt;=$F21+$G21-1),2,IF(AND($C21="Milestone",BL$7&gt;=$F21,BL$7&lt;=$F21+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="BM21" s="19"/>
     </row>
     <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="78" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="23"/>
@@ -5901,7 +5906,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="25"/>
       <c r="G22" s="26"/>
-      <c r="H22" s="53"/>
+      <c r="H22" s="52"/>
       <c r="I22" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -6148,7 +6153,7 @@
       <c r="G23" s="26">
         <v>6</v>
       </c>
-      <c r="H23" s="53"/>
+      <c r="H23" s="52"/>
       <c r="I23" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -6395,7 +6400,7 @@
       <c r="G24" s="26">
         <v>1</v>
       </c>
-      <c r="H24" s="53"/>
+      <c r="H24" s="52"/>
       <c r="I24" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -6500,9 +6505,9 @@
         <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
-      <c r="AI24" s="20" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
+      <c r="AI24" s="20">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
       </c>
       <c r="AJ24" s="20" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -6556,9 +6561,9 @@
         <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
-      <c r="AW24" s="20">
-        <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+      <c r="AW24" s="20" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v/>
       </c>
       <c r="AX24" s="20" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -6642,7 +6647,7 @@
       <c r="G25" s="26">
         <v>9</v>
       </c>
-      <c r="H25" s="53"/>
+      <c r="H25" s="52"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
@@ -6721,7 +6726,7 @@
       <c r="G26" s="26">
         <v>4</v>
       </c>
-      <c r="H26" s="53"/>
+      <c r="H26" s="52"/>
       <c r="I26" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -6851,39 +6856,39 @@
         <v/>
       </c>
       <c r="AO26" s="20" t="str">
-        <f t="shared" ref="AO26:AW26" ca="1" si="16">IF(AND($C26="Goal",AO$7&gt;=$F26,AO$7&lt;=$F26+$G26-1),2,IF(AND($C26="Milestone",AO$7&gt;=$F26,AO$7&lt;=$F26+$G26-1),1,""))</f>
+        <f t="shared" ref="AO26:AW26" ca="1" si="21">IF(AND($C26="Goal",AO$7&gt;=$F26,AO$7&lt;=$F26+$G26-1),2,IF(AND($C26="Milestone",AO$7&gt;=$F26,AO$7&lt;=$F26+$G26-1),1,""))</f>
         <v/>
       </c>
       <c r="AP26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AQ26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AR26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AS26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AT26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AU26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AV26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AW26" s="20" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AX26" s="20" t="str">
@@ -6968,7 +6973,7 @@
       <c r="G27" s="26">
         <v>1</v>
       </c>
-      <c r="H27" s="53"/>
+      <c r="H27" s="52"/>
       <c r="I27" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -7129,9 +7134,9 @@
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="AW27" s="20" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
+      <c r="AW27" s="20">
+        <f t="shared" ca="1" si="11"/>
+        <v>1</v>
       </c>
       <c r="AX27" s="20" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -7185,9 +7190,9 @@
         <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
-      <c r="BK27" s="20">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+      <c r="BK27" s="20" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
       </c>
       <c r="BL27" s="20" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -7215,7 +7220,7 @@
       <c r="G28" s="26">
         <v>5</v>
       </c>
-      <c r="H28" s="53"/>
+      <c r="H28" s="52"/>
       <c r="I28" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -7281,140 +7286,140 @@
         <v/>
       </c>
       <c r="Y28" s="20" t="str">
-        <f t="shared" ref="Y28:BD29" ca="1" si="17">IF(AND($C28="Goal",Y$7&gt;=$F28,Y$7&lt;=$F28+$G28-1),2,IF(AND($C28="Milestone",Y$7&gt;=$F28,Y$7&lt;=$F28+$G28-1),1,""))</f>
+        <f t="shared" ref="Y28:BD29" ca="1" si="22">IF(AND($C28="Goal",Y$7&gt;=$F28,Y$7&lt;=$F28+$G28-1),2,IF(AND($C28="Milestone",Y$7&gt;=$F28,Y$7&lt;=$F28+$G28-1),1,""))</f>
         <v/>
       </c>
       <c r="Z28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AA28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AB28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AC28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AD28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AE28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AF28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AG28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AH28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AI28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AJ28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AK28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AL28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AM28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AN28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AO28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AP28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AQ28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AR28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AS28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AT28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AU28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AV28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AW28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AX28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AY28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AZ28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="BA28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v/>
-      </c>
-      <c r="BB28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v/>
-      </c>
-      <c r="BC28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v/>
-      </c>
-      <c r="BD28" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v/>
-      </c>
-      <c r="BE28" s="20" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="BF28" s="20" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BB28" s="20">
+        <f t="shared" ca="1" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="BC28" s="20">
+        <f t="shared" ca="1" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="BD28" s="20">
+        <f t="shared" ca="1" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="BE28" s="20">
+        <f t="shared" ca="1" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="BF28" s="20">
+        <f t="shared" ca="1" si="12"/>
+        <v>2</v>
       </c>
       <c r="BG28" s="20" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -7462,7 +7467,7 @@
       <c r="G29" s="26">
         <v>11</v>
       </c>
-      <c r="H29" s="53"/>
+      <c r="H29" s="52"/>
       <c r="I29" s="20" t="str">
         <f t="shared" ca="1" si="13"/>
         <v/>
@@ -7592,31 +7597,31 @@
         <v/>
       </c>
       <c r="AO29" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AP29" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AQ29" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AR29" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AS29" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AT29" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AU29" s="20" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AV29" s="20" t="str">
@@ -7691,72 +7696,72 @@
     </row>
     <row r="30" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
-      <c r="B30" s="80" t="s">
+      <c r="B30" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="36"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="54"/>
-      <c r="U30" s="54"/>
-      <c r="V30" s="54"/>
-      <c r="W30" s="54"/>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="54"/>
-      <c r="Z30" s="54"/>
-      <c r="AA30" s="54"/>
-      <c r="AB30" s="54"/>
-      <c r="AC30" s="54"/>
-      <c r="AD30" s="54"/>
-      <c r="AE30" s="54"/>
-      <c r="AF30" s="54"/>
-      <c r="AG30" s="54"/>
-      <c r="AH30" s="54"/>
-      <c r="AI30" s="54"/>
-      <c r="AJ30" s="54"/>
-      <c r="AK30" s="54"/>
-      <c r="AL30" s="54"/>
-      <c r="AM30" s="54"/>
-      <c r="AN30" s="54"/>
-      <c r="AO30" s="54"/>
-      <c r="AP30" s="54"/>
-      <c r="AQ30" s="54"/>
-      <c r="AR30" s="54"/>
-      <c r="AS30" s="54"/>
-      <c r="AT30" s="54"/>
-      <c r="AU30" s="54"/>
-      <c r="AV30" s="54"/>
-      <c r="AW30" s="54"/>
-      <c r="AX30" s="54"/>
-      <c r="AY30" s="54"/>
-      <c r="AZ30" s="54"/>
-      <c r="BA30" s="54"/>
-      <c r="BB30" s="54"/>
-      <c r="BC30" s="54"/>
-      <c r="BD30" s="54"/>
-      <c r="BE30" s="54"/>
-      <c r="BF30" s="54"/>
-      <c r="BG30" s="54"/>
-      <c r="BH30" s="54"/>
-      <c r="BI30" s="54"/>
-      <c r="BJ30" s="54"/>
-      <c r="BK30" s="54"/>
-      <c r="BL30" s="54"/>
-      <c r="BM30" s="47"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="53"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="53"/>
+      <c r="X30" s="53"/>
+      <c r="Y30" s="53"/>
+      <c r="Z30" s="53"/>
+      <c r="AA30" s="53"/>
+      <c r="AB30" s="53"/>
+      <c r="AC30" s="53"/>
+      <c r="AD30" s="53"/>
+      <c r="AE30" s="53"/>
+      <c r="AF30" s="53"/>
+      <c r="AG30" s="53"/>
+      <c r="AH30" s="53"/>
+      <c r="AI30" s="53"/>
+      <c r="AJ30" s="53"/>
+      <c r="AK30" s="53"/>
+      <c r="AL30" s="53"/>
+      <c r="AM30" s="53"/>
+      <c r="AN30" s="53"/>
+      <c r="AO30" s="53"/>
+      <c r="AP30" s="53"/>
+      <c r="AQ30" s="53"/>
+      <c r="AR30" s="53"/>
+      <c r="AS30" s="53"/>
+      <c r="AT30" s="53"/>
+      <c r="AU30" s="53"/>
+      <c r="AV30" s="53"/>
+      <c r="AW30" s="53"/>
+      <c r="AX30" s="53"/>
+      <c r="AY30" s="53"/>
+      <c r="AZ30" s="53"/>
+      <c r="BA30" s="53"/>
+      <c r="BB30" s="53"/>
+      <c r="BC30" s="53"/>
+      <c r="BD30" s="53"/>
+      <c r="BE30" s="53"/>
+      <c r="BF30" s="53"/>
+      <c r="BG30" s="53"/>
+      <c r="BH30" s="53"/>
+      <c r="BI30" s="53"/>
+      <c r="BJ30" s="53"/>
+      <c r="BK30" s="53"/>
+      <c r="BL30" s="53"/>
+      <c r="BM30" s="46"/>
     </row>
     <row r="31" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
@@ -7789,6 +7794,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B2:AH2"/>
     <mergeCell ref="E4:H4"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="X4:AA4"/>
@@ -7796,7 +7802,6 @@
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:V4"/>
-    <mergeCell ref="B2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E12 E17 E30 E22:E27">
     <cfRule type="dataBar" priority="28">
@@ -7813,56 +7818,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL30">
-    <cfRule type="expression" dxfId="13" priority="24">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="12" priority="27">
+    <cfRule type="expression" dxfId="20" priority="27">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="11" priority="26">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="10" priority="25">
+    <cfRule type="expression" dxfId="18" priority="25">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL29">
-    <cfRule type="expression" dxfId="9" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="30" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="31" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="32" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="33" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="34" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BL30">
-    <cfRule type="expression" dxfId="4" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="36" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="37" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="38" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="39" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="40" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8082,20 +8087,23 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Project information starting in cell B11 through cell G11. _x000a_Enter Milestone Description, select a Category, assign someone to the task, and enter the progress, start date, and number of days for the task to start charting._x000a_" sqref="A11" xr:uid="{77315CCB-C571-42B0-8983-9C17BB04F75F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Gantt milestone data. DO NOT enter anything in this row. _x000a_To add more items, insert new rows above this one._x000a_" sqref="A30" xr:uid="{659FD5CB-B62B-4854-B8A9-29F1F70930AC}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{48C85E0F-C5AB-4EEB-8324-B04F96DA2F78}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="16385" r:id="rId4" name="Scroll Bar 1">
+            <control shapeId="16385" r:id="rId5" name="Scroll Bar 1">
               <controlPr defaultSize="0" autoPict="0" altText="Scroll bar to scroll through the Ghantt project timeline.">
                 <anchor moveWithCells="1">
                   <from>
@@ -8119,7 +8127,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -8138,44 +8146,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>E9:E12 E17 E30 E22:E27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="35" id="{A1EFF969-3CBB-4DB2-A4C9-47B01FE32C86}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>I30:BL30</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="50" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>I10:BL29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CC885458-7685-472F-BE7A-D937EA312539}">
@@ -8386,6 +8356,44 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>E20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="35" id="{A1EFF969-3CBB-4DB2-A4C9-47B01FE32C86}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I30:BL30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="50" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I10:BL29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>